<commit_message>
Rephrased to dynamic elements
</commit_message>
<xml_diff>
--- a/domaingroups/Beta-Prop/e4v6wAg1_results.xlsx
+++ b/domaingroups/Beta-Prop/e4v6wAg1_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bounedutr-my.sharepoint.com/personal/yigit_kutlu_boun_edu_tr/Documents/Themes&amp;Dynamics/New Domains/Calculations/Beta-Prop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bounedutr-my.sharepoint.com/personal/yigit_kutlu_bounedutr_onmicrosoft_com/Documents/Themes&amp;Dynamics/WebSiteFiles/Beta-Prop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC10481D999E7FD05ADE58E0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE2A83F-BA01-48D4-BB33-6B603C29EE0D}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_F25DC773A252ABDACC10481D999E7FD05ADE58E0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6595C08F-6290-43FF-A2F6-D12F8A689320}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Index</t>
-  </si>
-  <si>
-    <t>Dynamic Domains</t>
   </si>
   <si>
     <t>Theme Combinations</t>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>Mode-7</t>
+  </si>
+  <si>
+    <t>Dynamic Elements</t>
   </si>
 </sst>
 </file>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="AA186" sqref="AA186"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,16 +695,16 @@
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="I1" s="6"/>
       <c r="P1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
       <c r="Y1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z1" s="8"/>
       <c r="AA1" s="8"/>
@@ -714,7 +714,7 @@
       <c r="AE1" s="8"/>
       <c r="AF1" s="8"/>
       <c r="AG1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AH1" s="8"/>
       <c r="AI1" s="8"/>
@@ -724,12 +724,12 @@
       <c r="AM1" s="8"/>
       <c r="AN1" s="8"/>
       <c r="AO1" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -741,25 +741,25 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -769,69 +769,69 @@
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AC2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AE2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AF2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AG2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AH2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AI2" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="AI2" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="AJ2" s="8"/>
       <c r="AK2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AM2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AN2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AO2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AP2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AP2" s="8" t="s">
+      <c r="AQ2" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="AQ2" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="AR2" s="8"/>
       <c r="AS2" s="8"/>
@@ -844,7 +844,7 @@
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>58</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>58</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>59</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>59</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>60</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>62</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>72</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>104</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>109</v>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>112</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>119</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>166</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>166</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19">
         <v>166</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>166</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>188</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>217</v>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>219</v>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>229</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>233</v>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>237</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>266</v>
@@ -3324,7 +3324,7 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>277</v>
@@ -3419,7 +3419,7 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>18</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32">
         <v>59</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33">
         <v>62</v>
@@ -3873,7 +3873,7 @@
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>94</v>
@@ -3965,7 +3965,7 @@
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35">
         <v>100</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36">
         <v>101</v>
@@ -4149,7 +4149,7 @@
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37">
         <v>104</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>146</v>
@@ -4333,7 +4333,7 @@
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>146</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40">
         <v>147</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <v>75</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42">
         <v>191</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43">
         <v>191</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44">
         <v>191</v>
@@ -4885,7 +4885,7 @@
     </row>
     <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45">
         <v>196</v>
@@ -4977,7 +4977,7 @@
     </row>
     <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46">
         <v>196</v>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47">
         <v>256</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N48">
         <v>2</v>
@@ -5247,7 +5247,7 @@
     </row>
     <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -5339,7 +5339,7 @@
     </row>
     <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50">
         <v>75</v>
@@ -5431,7 +5431,7 @@
     </row>
     <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51">
         <v>109</v>
@@ -5523,7 +5523,7 @@
     </row>
     <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52">
         <v>146</v>
@@ -16156,7 +16156,7 @@
     </row>
     <row r="181" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S181" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U181">
         <v>1.3893</v>
@@ -16224,12 +16224,12 @@
     </row>
     <row r="183" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S183" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="184" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S184" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U184">
         <v>0.9556</v>
@@ -16255,7 +16255,7 @@
     </row>
     <row r="185" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S185" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U185">
         <v>0.222</v>
@@ -16281,7 +16281,7 @@
     </row>
     <row r="186" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S186" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U186">
         <v>2.5499999999999998E-2</v>
@@ -16307,7 +16307,7 @@
     </row>
     <row r="187" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S187" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U187">
         <v>6.58</v>
@@ -16315,7 +16315,7 @@
     </row>
     <row r="188" spans="14:43" x14ac:dyDescent="0.25">
       <c r="S188" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U188">
         <v>250</v>

</xml_diff>